<commit_message>
added results for logistic regression
</commit_message>
<xml_diff>
--- a/win_comparisons.xlsx
+++ b/win_comparisons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencer/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencer/Dropbox/PROJECTS/NFL/ML_TESTING/ML_Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Week</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>RFC Best Score:</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
   </si>
 </sst>
 </file>
@@ -140,13 +143,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -426,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
@@ -1060,43 +1062,43 @@
         <v>3</v>
       </c>
       <c r="B20" s="3">
-        <f>SUM(B3:B18)</f>
+        <f t="shared" ref="B20:K20" si="0">SUM(B3:B18)</f>
         <v>41</v>
       </c>
       <c r="C20" s="3">
-        <f>SUM(C3:C18)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="D20" s="3">
-        <f>SUM(D3:D18)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="E20" s="3">
-        <f>SUM(E3:E18)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="F20" s="3">
-        <f>SUM(F3:F18)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="G20" s="3">
-        <f>SUM(G3:G18)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="H20" s="3">
-        <f>SUM(H3:H18)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="I20" s="3">
-        <f>SUM(I3:I18)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="J20" s="3">
-        <f>SUM(J3:J18)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="K20" s="3">
-        <f>SUM(K3:K18)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
@@ -1170,17 +1172,650 @@
         <v>0.51046000000000002</v>
       </c>
     </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <f>SUM(B26:B41)</f>
+        <v>36</v>
+      </c>
+      <c r="C43">
+        <f>SUM(C26:C41)</f>
+        <v>28</v>
+      </c>
+      <c r="D43">
+        <f>SUM(D26:D41)</f>
+        <v>38</v>
+      </c>
+      <c r="E43">
+        <f>SUM(E26:E41)</f>
+        <v>36</v>
+      </c>
+      <c r="F43">
+        <f>SUM(F26:F41)</f>
+        <v>41</v>
+      </c>
+      <c r="G43">
+        <f>SUM(G26:G41)</f>
+        <v>44</v>
+      </c>
+      <c r="H43">
+        <f>SUM(H26:H41)</f>
+        <v>47</v>
+      </c>
+      <c r="I43">
+        <f>SUM(I26:I41)</f>
+        <v>47</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J26:J41)</f>
+        <v>47</v>
+      </c>
+      <c r="K43">
+        <f>SUM(K26:K41)</f>
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>